<commit_message>
planilha de homologação e att do doc final @brunagd
</commit_message>
<xml_diff>
--- a/Documentação/planilha de homologação.xlsx
+++ b/Documentação/planilha de homologação.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bunag\Desktop\control-block\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\control-block\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBAF0FB-49D1-42FD-8916-0CD01E68839C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
@@ -23,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>move0011</author>
   </authors>
   <commentList>
-    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="154">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -517,7 +516,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
@@ -1583,11 +1582,181 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="20" xfId="15" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="28" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="29" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="30" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="31" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="32" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="33" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1637,153 +1806,6 @@
     <xf numFmtId="0" fontId="33" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="28" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="29" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="30" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="31" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="32" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="33" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="20" xfId="15" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1815,47 +1837,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="Background" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Background" xfId="1"/>
     <cellStyle name="Cálculo" xfId="15" builtinId="22"/>
-    <cellStyle name="Card" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Card B" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Card BL" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Card BR" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Card L" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Card R" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Card T" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Card TL" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Card TR" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Column Header" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Card" xfId="2"/>
+    <cellStyle name="Card B" xfId="3"/>
+    <cellStyle name="Card BL" xfId="4"/>
+    <cellStyle name="Card BR" xfId="5"/>
+    <cellStyle name="Card L" xfId="6"/>
+    <cellStyle name="Card R" xfId="7"/>
+    <cellStyle name="Card T" xfId="8"/>
+    <cellStyle name="Card TL" xfId="9"/>
+    <cellStyle name="Card TR" xfId="10"/>
+    <cellStyle name="Column Header" xfId="11"/>
     <cellStyle name="Hiperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="Input" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Input" xfId="13"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2" xfId="14"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1938,6 +1937,928 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1796144</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1036114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11498037" y="7184572"/>
+          <a:ext cx="1415143" cy="900042"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>408215</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>204108</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1713287</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1034144</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11525251" y="6109608"/>
+          <a:ext cx="1305072" cy="830036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>557893</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>54430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1700893</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>462644</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11674929" y="8817430"/>
+          <a:ext cx="1143000" cy="408214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>16329</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>193223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1321401</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1023259</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16385722" y="7241723"/>
+          <a:ext cx="1305072" cy="830036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>112008</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>166008</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1348615</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16481401" y="6071508"/>
+          <a:ext cx="1236607" cy="786492"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1362223</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>489856</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16426544" y="8806543"/>
+          <a:ext cx="1305072" cy="446313"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>264140</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1219201</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>544287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16633533" y="8218715"/>
+          <a:ext cx="955061" cy="517072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>661469</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>29936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1616530</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>547008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11778505" y="8221436"/>
+          <a:ext cx="955061" cy="517072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>680357</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1460871</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1034143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11797393" y="4912178"/>
+          <a:ext cx="780514" cy="884465"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>340178</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1204746</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1074963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16709571" y="4857749"/>
+          <a:ext cx="864568" cy="979714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>693965</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1568710</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1238250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811001" y="4912179"/>
+          <a:ext cx="874745" cy="1088571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>751115</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>84365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1046177</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11868151" y="6180365"/>
+          <a:ext cx="772885" cy="961812"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>693965</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1568710</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811001" y="7293429"/>
+          <a:ext cx="874745" cy="1088571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>272143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1686072</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1102179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11498036" y="8654143"/>
+          <a:ext cx="1305072" cy="830036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>421822</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1726894</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1020535</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11538858" y="9905999"/>
+          <a:ext cx="1305072" cy="830036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>816429</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1564822</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>340179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11933465" y="10912929"/>
+          <a:ext cx="748393" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>802821</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>81644</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1583335</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>367394</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11919857" y="11321144"/>
+          <a:ext cx="780514" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>288472</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>125186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1163217</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1213757</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16657865" y="4887686"/>
+          <a:ext cx="874745" cy="1088571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1141057</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1115786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16723179" y="6232071"/>
+          <a:ext cx="787271" cy="979715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>410937</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1152285</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1088573</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16780330" y="7405007"/>
+          <a:ext cx="741348" cy="922566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>342901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1348615</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1172937</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16412936" y="8724901"/>
+          <a:ext cx="1305072" cy="830036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>46265</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>168730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1351337</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>998766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagem 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16415658" y="9884230"/>
+          <a:ext cx="1305072" cy="830036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>302080</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>29936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1050473</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>315686</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagem 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16671473" y="10888436"/>
+          <a:ext cx="748393" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>397329</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>84365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1177843</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>370115</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagem 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16766722" y="11323865"/>
+          <a:ext cx="780514" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -2014,23 +2935,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2066,23 +2970,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2258,7 +3145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -2299,13 +3186,13 @@
     </row>
     <row r="2" spans="1:20" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="49"/>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="104"/>
       <c r="G2" s="70"/>
       <c r="H2" s="52"/>
       <c r="I2" s="52"/>
@@ -2315,11 +3202,11 @@
     </row>
     <row r="3" spans="1:20" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="49"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="106"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="107"/>
       <c r="G3" s="70"/>
       <c r="H3" s="52"/>
       <c r="I3" s="52"/>
@@ -2346,10 +3233,10 @@
       <c r="B5" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="107" t="s">
+      <c r="C5" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="108"/>
+      <c r="D5" s="109"/>
       <c r="E5" s="25"/>
       <c r="F5" s="26"/>
       <c r="G5" s="25"/>
@@ -2364,10 +3251,10 @@
       <c r="B6" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="107">
+      <c r="C6" s="108">
         <v>1</v>
       </c>
-      <c r="D6" s="108"/>
+      <c r="D6" s="109"/>
       <c r="E6" s="25"/>
       <c r="F6" s="26"/>
       <c r="G6" s="25"/>
@@ -2382,10 +3269,10 @@
       <c r="B7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="108"/>
+      <c r="D7" s="109"/>
       <c r="E7" s="25"/>
       <c r="F7" s="26"/>
       <c r="G7" s="25"/>
@@ -2400,10 +3287,10 @@
       <c r="B8" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="108"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="25"/>
       <c r="F8" s="26"/>
       <c r="G8" s="25"/>
@@ -2418,10 +3305,10 @@
       <c r="B9" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="111">
+      <c r="C9" s="112">
         <v>43777</v>
       </c>
-      <c r="D9" s="112"/>
+      <c r="D9" s="113"/>
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>
       <c r="G9" s="25"/>
@@ -2447,14 +3334,14 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="113"/>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="115"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="116"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="22"/>
@@ -2466,14 +3353,14 @@
       <c r="B12" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="75" t="s">
+      <c r="D12" s="120"/>
+      <c r="E12" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="76"/>
+      <c r="F12" s="120"/>
       <c r="G12" s="64" t="s">
         <v>23</v>
       </c>
@@ -2496,14 +3383,14 @@
       <c r="B13" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="110"/>
-      <c r="E13" s="116" t="s">
+      <c r="D13" s="111"/>
+      <c r="E13" s="121" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="117"/>
+      <c r="F13" s="122"/>
       <c r="G13" s="58"/>
       <c r="H13" s="65">
         <v>43789</v>
@@ -2524,14 +3411,14 @@
       <c r="B14" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="87"/>
-      <c r="E14" s="118" t="s">
+      <c r="D14" s="135"/>
+      <c r="E14" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="119"/>
+      <c r="F14" s="124"/>
       <c r="G14" s="58"/>
       <c r="H14" s="65">
         <v>43789</v>
@@ -2552,14 +3439,14 @@
       <c r="B15" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="82" t="s">
+      <c r="D15" s="137"/>
+      <c r="E15" s="130" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="83"/>
+      <c r="F15" s="131"/>
       <c r="G15" s="58"/>
       <c r="H15" s="65">
         <v>43789</v>
@@ -2600,17 +3487,17 @@
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="51"/>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="133"/>
+      <c r="J19" s="133"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="R19" s="5"/>
@@ -2623,18 +3510,18 @@
       <c r="B20" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="90" t="s">
+      <c r="C20" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="91"/>
-      <c r="E20" s="90" t="s">
+      <c r="D20" s="118"/>
+      <c r="E20" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="91"/>
-      <c r="G20" s="90" t="s">
+      <c r="F20" s="118"/>
+      <c r="G20" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="91"/>
+      <c r="H20" s="118"/>
       <c r="I20" s="63" t="s">
         <v>25</v>
       </c>
@@ -2653,18 +3540,18 @@
       <c r="B21" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="79"/>
-      <c r="E21" s="78" t="s">
+      <c r="D21" s="127"/>
+      <c r="E21" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="79"/>
-      <c r="G21" s="129" t="s">
+      <c r="F21" s="127"/>
+      <c r="G21" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="130"/>
+      <c r="H21" s="86"/>
       <c r="I21" s="72" t="s">
         <v>89</v>
       </c>
@@ -2683,18 +3570,18 @@
       <c r="B22" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80" t="s">
+      <c r="D22" s="127"/>
+      <c r="E22" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="81"/>
-      <c r="G22" s="77" t="s">
+      <c r="F22" s="129"/>
+      <c r="G22" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="77"/>
+      <c r="H22" s="125"/>
       <c r="I22" s="72" t="s">
         <v>89</v>
       </c>
@@ -2713,18 +3600,18 @@
       <c r="B23" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="78" t="s">
+      <c r="C23" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="80" t="s">
+      <c r="D23" s="127"/>
+      <c r="E23" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="81"/>
-      <c r="G23" s="77" t="s">
+      <c r="F23" s="129"/>
+      <c r="G23" s="125" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="77"/>
+      <c r="H23" s="125"/>
       <c r="I23" s="72" t="s">
         <v>89</v>
       </c>
@@ -2736,25 +3623,25 @@
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="50"/>
-      <c r="B24" s="120" t="s">
+      <c r="B24" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="124"/>
-      <c r="E24" s="123" t="s">
+      <c r="D24" s="91"/>
+      <c r="E24" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="124"/>
-      <c r="G24" s="95" t="s">
+      <c r="F24" s="91"/>
+      <c r="G24" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="H24" s="96"/>
-      <c r="I24" s="92" t="s">
+      <c r="H24" s="97"/>
+      <c r="I24" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="J24" s="92" t="s">
+      <c r="J24" s="82" t="s">
         <v>90</v>
       </c>
       <c r="K24" s="25"/>
@@ -2762,81 +3649,81 @@
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="126"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="98"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="83"/>
       <c r="K25" s="25"/>
       <c r="L25" s="22"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
-      <c r="B26" s="121"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="93"/>
-      <c r="J26" s="93"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="83"/>
       <c r="K26" s="25"/>
       <c r="L26" s="22"/>
     </row>
     <row r="27" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
-      <c r="B27" s="121"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="126"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="93"/>
-      <c r="J27" s="93"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="83"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
     </row>
     <row r="28" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="128"/>
-      <c r="E28" s="127"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="94"/>
-      <c r="J28" s="94"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
     </row>
     <row r="29" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
-      <c r="B29" s="120" t="s">
+      <c r="B29" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="123" t="s">
+      <c r="C29" s="90" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="124"/>
-      <c r="E29" s="123" t="s">
+      <c r="D29" s="91"/>
+      <c r="E29" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="124"/>
-      <c r="G29" s="95" t="s">
+      <c r="F29" s="91"/>
+      <c r="G29" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="H29" s="96"/>
-      <c r="I29" s="92" t="s">
+      <c r="H29" s="97"/>
+      <c r="I29" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="J29" s="92" t="s">
+      <c r="J29" s="82" t="s">
         <v>90</v>
       </c>
       <c r="K29" s="22"/>
@@ -2844,187 +3731,187 @@
     </row>
     <row r="30" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
-      <c r="B30" s="121"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="98"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
     </row>
     <row r="31" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
-      <c r="B31" s="121"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="126"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
     </row>
     <row r="32" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="121"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="93"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="83"/>
     </row>
     <row r="33" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="122"/>
-      <c r="C33" s="127"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="128"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="84"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="120" t="s">
+      <c r="B34" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="123" t="s">
+      <c r="C34" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="124"/>
-      <c r="E34" s="123" t="s">
+      <c r="D34" s="91"/>
+      <c r="E34" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="124"/>
-      <c r="G34" s="95" t="s">
+      <c r="F34" s="91"/>
+      <c r="G34" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="96"/>
-      <c r="I34" s="92" t="s">
+      <c r="H34" s="97"/>
+      <c r="I34" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="J34" s="92" t="s">
+      <c r="J34" s="82" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="121"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="126"/>
-      <c r="E35" s="125"/>
-      <c r="F35" s="126"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="98"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="121"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="126"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="92"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="121"/>
-      <c r="C37" s="125"/>
-      <c r="D37" s="126"/>
-      <c r="E37" s="125"/>
-      <c r="F37" s="126"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="98"/>
-      <c r="I37" s="93"/>
-      <c r="J37" s="93"/>
+      <c r="B37" s="88"/>
+      <c r="C37" s="92"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="98"/>
+      <c r="H37" s="99"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="122"/>
-      <c r="C38" s="127"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="127"/>
-      <c r="F38" s="128"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="100"/>
-      <c r="I38" s="94"/>
-      <c r="J38" s="94"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="95"/>
+      <c r="G38" s="100"/>
+      <c r="H38" s="101"/>
+      <c r="I38" s="84"/>
+      <c r="J38" s="84"/>
     </row>
     <row r="39" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="120" t="s">
+      <c r="B39" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="124"/>
-      <c r="E39" s="123" t="s">
+      <c r="D39" s="91"/>
+      <c r="E39" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="124"/>
-      <c r="G39" s="95" t="s">
+      <c r="F39" s="91"/>
+      <c r="G39" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="H39" s="96"/>
-      <c r="I39" s="92" t="s">
+      <c r="H39" s="97"/>
+      <c r="I39" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="J39" s="92" t="s">
+      <c r="J39" s="82" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="121"/>
-      <c r="C40" s="125"/>
-      <c r="D40" s="126"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="126"/>
-      <c r="G40" s="97"/>
-      <c r="H40" s="98"/>
-      <c r="I40" s="93"/>
-      <c r="J40" s="93"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="99"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="83"/>
     </row>
     <row r="41" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="121"/>
-      <c r="C41" s="125"/>
-      <c r="D41" s="126"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="97"/>
-      <c r="H41" s="98"/>
-      <c r="I41" s="93"/>
-      <c r="J41" s="93"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="98"/>
+      <c r="H41" s="99"/>
+      <c r="I41" s="83"/>
+      <c r="J41" s="83"/>
     </row>
     <row r="42" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="121"/>
-      <c r="C42" s="125"/>
-      <c r="D42" s="126"/>
-      <c r="E42" s="125"/>
-      <c r="F42" s="126"/>
-      <c r="G42" s="97"/>
-      <c r="H42" s="98"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="99"/>
+      <c r="I42" s="83"/>
+      <c r="J42" s="83"/>
     </row>
     <row r="43" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="122"/>
-      <c r="C43" s="127"/>
-      <c r="D43" s="128"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="128"/>
-      <c r="G43" s="99"/>
-      <c r="H43" s="100"/>
-      <c r="I43" s="94"/>
-      <c r="J43" s="94"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="95"/>
+      <c r="G43" s="100"/>
+      <c r="H43" s="101"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="84"/>
     </row>
     <row r="55" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B55" s="56" t="s">
@@ -3040,6 +3927,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="G24:H28"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:D33"/>
+    <mergeCell ref="E29:F33"/>
+    <mergeCell ref="G29:H33"/>
+    <mergeCell ref="E24:F28"/>
+    <mergeCell ref="C24:D28"/>
     <mergeCell ref="I29:I33"/>
     <mergeCell ref="J29:J33"/>
     <mergeCell ref="G21:H21"/>
@@ -3056,53 +3980,16 @@
     <mergeCell ref="J34:J38"/>
     <mergeCell ref="J39:J43"/>
     <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:D33"/>
-    <mergeCell ref="E29:F33"/>
-    <mergeCell ref="G29:H33"/>
-    <mergeCell ref="E24:F28"/>
-    <mergeCell ref="C24:D28"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="G24:H28"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I15">
       <formula1>"Não Iniciado, Em andamento, Concluído, Pendente"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J21:J24 J29 J34 J39" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J21:J24 J29 J34 J39">
       <formula1>"Não testado,Testado- NÃO OK,Testado - OK"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I21:I24 I29 I34 I39" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I21:I24 I29 I34 I39">
       <formula1>"Essencial, Importante, Desejável"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3113,11 +4000,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3220,10 +4107,10 @@
       <c r="A15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="138" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="131"/>
+      <c r="C15" s="138"/>
       <c r="D15" s="38"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3297,9 +4184,7 @@
       <c r="H25" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="48" t="s">
-        <v>45</v>
-      </c>
+      <c r="I25" s="48"/>
       <c r="Q25" s="41"/>
       <c r="R25" s="41"/>
       <c r="S25" s="41"/>
@@ -3328,9 +4213,7 @@
       <c r="H26" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="I26" s="48" t="s">
-        <v>45</v>
-      </c>
+      <c r="I26" s="48"/>
       <c r="Q26" s="41"/>
       <c r="R26" s="41"/>
       <c r="S26" s="41"/>
@@ -3359,9 +4242,7 @@
       <c r="H27" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="I27" s="48" t="s">
-        <v>45</v>
-      </c>
+      <c r="I27" s="48"/>
       <c r="Q27" s="41"/>
       <c r="R27" s="41"/>
       <c r="S27" s="41"/>
@@ -3390,9 +4271,7 @@
       <c r="H28" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="48" t="s">
-        <v>45</v>
-      </c>
+      <c r="I28" s="48"/>
       <c r="Q28" s="41"/>
       <c r="R28" s="41"/>
       <c r="S28" s="41"/>
@@ -3421,9 +4300,7 @@
       <c r="H29" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="48" t="s">
-        <v>45</v>
-      </c>
+      <c r="I29" s="48"/>
       <c r="Q29" s="41"/>
       <c r="R29" s="41"/>
       <c r="S29" s="41"/>
@@ -3514,11 +4391,12 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -3539,20 +4417,20 @@
     <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="60"/>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="141"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="135"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="137"/>
+      <c r="B3" s="142"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="144"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -3560,19 +4438,19 @@
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="142" t="s">
+      <c r="B5" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="143" t="s">
+      <c r="C5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="145" t="s">
+      <c r="E5" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="146" t="s">
+      <c r="F5" s="80" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3714,30 +4592,30 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="14"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="145"/>
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="146" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="140"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="147"/>
+      <c r="F16" s="147"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="139"/>
+      <c r="B17" s="146"/>
       <c r="C17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="147"/>
+      <c r="F17" s="147"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B20" s="12"/>
@@ -3880,11 +4758,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FBE274-996E-4EA2-A2ED-177DACC54553}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="B22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3987,10 +4865,10 @@
       <c r="A15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="138" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="131"/>
+      <c r="C15" s="138"/>
       <c r="D15" s="73"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -4042,7 +4920,7 @@
       <c r="T24" s="41"/>
     </row>
     <row r="25" spans="1:20" s="40" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A25" s="147" t="s">
+      <c r="A25" s="81" t="s">
         <v>133</v>
       </c>
       <c r="B25" s="39" t="s">
@@ -4073,7 +4951,7 @@
       <c r="T25" s="41"/>
     </row>
     <row r="26" spans="1:20" s="40" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="81" t="s">
         <v>134</v>
       </c>
       <c r="B26" s="39" t="s">
@@ -4104,7 +4982,7 @@
       <c r="T26" s="41"/>
     </row>
     <row r="27" spans="1:20" s="40" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A27" s="147" t="s">
+      <c r="A27" s="81" t="s">
         <v>144</v>
       </c>
       <c r="B27" s="39" t="s">
@@ -4135,7 +5013,7 @@
       <c r="T27" s="41"/>
     </row>
     <row r="28" spans="1:20" s="40" customFormat="1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A28" s="147" t="s">
+      <c r="A28" s="81" t="s">
         <v>131</v>
       </c>
       <c r="B28" s="39" t="s">
@@ -4166,7 +5044,7 @@
       <c r="T28" s="41"/>
     </row>
     <row r="29" spans="1:20" s="40" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A29" s="147" t="s">
+      <c r="A29" s="81" t="s">
         <v>132</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -4197,7 +5075,7 @@
       <c r="T29" s="41"/>
     </row>
     <row r="30" spans="1:20" s="40" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="147" t="s">
+      <c r="A30" s="81" t="s">
         <v>147</v>
       </c>
       <c r="B30" s="39" t="s">
@@ -4228,7 +5106,7 @@
       <c r="T30" s="41"/>
     </row>
     <row r="31" spans="1:20" s="40" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="147" t="s">
+      <c r="A31" s="81" t="s">
         <v>138</v>
       </c>
       <c r="B31" s="39" t="s">
@@ -4240,7 +5118,7 @@
       <c r="D31" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="141" t="s">
+      <c r="E31" s="75" t="s">
         <v>141</v>
       </c>
       <c r="F31" s="43"/>
@@ -4322,5 +5200,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
att ptt e doc
</commit_message>
<xml_diff>
--- a/Documentação/planilha de homologação.xlsx
+++ b/Documentação/planilha de homologação.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -511,6 +511,9 @@
   </si>
   <si>
     <t>Abrir o site www.controblock.com, selecionar a opção/menu Cadastro; digitar Senha do usuário no  campo Senha; ir para o botão de cadastro</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1605,6 +1608,66 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1614,50 +1677,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="20" xfId="15" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1731,18 +1750,6 @@
     <xf numFmtId="0" fontId="17" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1758,53 +1765,49 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="33" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="20" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="20" xfId="15" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -3148,7 +3151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
@@ -3186,13 +3189,13 @@
     </row>
     <row r="2" spans="1:20" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="49"/>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="104"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="110"/>
       <c r="G2" s="70"/>
       <c r="H2" s="52"/>
       <c r="I2" s="52"/>
@@ -3202,11 +3205,11 @@
     </row>
     <row r="3" spans="1:20" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="49"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="107"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="113"/>
       <c r="G3" s="70"/>
       <c r="H3" s="52"/>
       <c r="I3" s="52"/>
@@ -3233,10 +3236,10 @@
       <c r="B5" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="109"/>
+      <c r="D5" s="115"/>
       <c r="E5" s="25"/>
       <c r="F5" s="26"/>
       <c r="G5" s="25"/>
@@ -3251,10 +3254,10 @@
       <c r="B6" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="114">
         <v>1</v>
       </c>
-      <c r="D6" s="109"/>
+      <c r="D6" s="115"/>
       <c r="E6" s="25"/>
       <c r="F6" s="26"/>
       <c r="G6" s="25"/>
@@ -3269,10 +3272,10 @@
       <c r="B7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="109"/>
+      <c r="D7" s="115"/>
       <c r="E7" s="25"/>
       <c r="F7" s="26"/>
       <c r="G7" s="25"/>
@@ -3287,10 +3290,10 @@
       <c r="B8" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="109"/>
+      <c r="D8" s="115"/>
       <c r="E8" s="25"/>
       <c r="F8" s="26"/>
       <c r="G8" s="25"/>
@@ -3305,10 +3308,10 @@
       <c r="B9" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="112">
+      <c r="C9" s="118">
         <v>43777</v>
       </c>
-      <c r="D9" s="113"/>
+      <c r="D9" s="119"/>
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>
       <c r="G9" s="25"/>
@@ -3334,14 +3337,14 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="114"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="116"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="122"/>
       <c r="J11" s="25"/>
       <c r="K11" s="25"/>
       <c r="L11" s="22"/>
@@ -3353,14 +3356,14 @@
       <c r="B12" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="119" t="s">
+      <c r="D12" s="83"/>
+      <c r="E12" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="120"/>
+      <c r="F12" s="83"/>
       <c r="G12" s="64" t="s">
         <v>23</v>
       </c>
@@ -3383,14 +3386,14 @@
       <c r="B13" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="111"/>
-      <c r="E13" s="121" t="s">
+      <c r="D13" s="117"/>
+      <c r="E13" s="123" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="122"/>
+      <c r="F13" s="124"/>
       <c r="G13" s="58"/>
       <c r="H13" s="65">
         <v>43789</v>
@@ -3411,14 +3414,14 @@
       <c r="B14" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="135"/>
-      <c r="E14" s="123" t="s">
+      <c r="D14" s="94"/>
+      <c r="E14" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="124"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="58"/>
       <c r="H14" s="65">
         <v>43789</v>
@@ -3439,14 +3442,14 @@
       <c r="B15" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="136" t="s">
+      <c r="C15" s="95" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="137"/>
-      <c r="E15" s="130" t="s">
+      <c r="D15" s="96"/>
+      <c r="E15" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="131"/>
+      <c r="F15" s="90"/>
       <c r="G15" s="58"/>
       <c r="H15" s="65">
         <v>43789</v>
@@ -3487,17 +3490,17 @@
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="51"/>
-      <c r="B19" s="132" t="s">
+      <c r="B19" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="133"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133"/>
-      <c r="F19" s="133"/>
-      <c r="G19" s="133"/>
-      <c r="H19" s="133"/>
-      <c r="I19" s="133"/>
-      <c r="J19" s="133"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="92"/>
+      <c r="J19" s="92"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="R19" s="5"/>
@@ -3510,18 +3513,18 @@
       <c r="B20" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="117" t="s">
+      <c r="C20" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="118"/>
-      <c r="E20" s="117" t="s">
+      <c r="D20" s="98"/>
+      <c r="E20" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="118"/>
-      <c r="G20" s="117" t="s">
+      <c r="F20" s="98"/>
+      <c r="G20" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="118"/>
+      <c r="H20" s="98"/>
       <c r="I20" s="63" t="s">
         <v>25</v>
       </c>
@@ -3540,18 +3543,18 @@
       <c r="B21" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="126" t="s">
+      <c r="C21" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="127"/>
-      <c r="E21" s="126" t="s">
+      <c r="D21" s="86"/>
+      <c r="E21" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="127"/>
-      <c r="G21" s="85" t="s">
+      <c r="F21" s="86"/>
+      <c r="G21" s="136" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="86"/>
+      <c r="H21" s="137"/>
       <c r="I21" s="72" t="s">
         <v>89</v>
       </c>
@@ -3570,18 +3573,18 @@
       <c r="B22" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="127"/>
-      <c r="E22" s="128" t="s">
+      <c r="D22" s="86"/>
+      <c r="E22" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="129"/>
-      <c r="G22" s="125" t="s">
+      <c r="F22" s="88"/>
+      <c r="G22" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="125"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="72" t="s">
         <v>89</v>
       </c>
@@ -3600,18 +3603,18 @@
       <c r="B23" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="127"/>
-      <c r="E23" s="128" t="s">
+      <c r="D23" s="86"/>
+      <c r="E23" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="129"/>
-      <c r="G23" s="125" t="s">
+      <c r="F23" s="88"/>
+      <c r="G23" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="125"/>
+      <c r="H23" s="84"/>
       <c r="I23" s="72" t="s">
         <v>89</v>
       </c>
@@ -3623,25 +3626,25 @@
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="50"/>
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="90" t="s">
+      <c r="C24" s="130" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="91"/>
-      <c r="E24" s="90" t="s">
+      <c r="D24" s="131"/>
+      <c r="E24" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="91"/>
-      <c r="G24" s="96" t="s">
+      <c r="F24" s="131"/>
+      <c r="G24" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="H24" s="97"/>
-      <c r="I24" s="82" t="s">
+      <c r="H24" s="103"/>
+      <c r="I24" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="J24" s="82" t="s">
+      <c r="J24" s="99" t="s">
         <v>90</v>
       </c>
       <c r="K24" s="25"/>
@@ -3649,81 +3652,81 @@
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="99"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="83"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
       <c r="K25" s="25"/>
       <c r="L25" s="22"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="98"/>
-      <c r="H26" s="99"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="83"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="133"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
       <c r="K26" s="25"/>
       <c r="L26" s="22"/>
     </row>
     <row r="27" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="99"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="83"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="133"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
     </row>
     <row r="28" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="101"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
     </row>
     <row r="29" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="90" t="s">
+      <c r="C29" s="130" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="91"/>
-      <c r="E29" s="90" t="s">
+      <c r="D29" s="131"/>
+      <c r="E29" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="91"/>
-      <c r="G29" s="96" t="s">
+      <c r="F29" s="131"/>
+      <c r="G29" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="H29" s="97"/>
-      <c r="I29" s="82" t="s">
+      <c r="H29" s="103"/>
+      <c r="I29" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="J29" s="82" t="s">
+      <c r="J29" s="99" t="s">
         <v>90</v>
       </c>
       <c r="K29" s="22"/>
@@ -3731,187 +3734,187 @@
     </row>
     <row r="30" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="98"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
+      <c r="B30" s="128"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="105"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="100"/>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
     </row>
     <row r="31" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="105"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
     </row>
     <row r="32" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="88"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="132"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
     </row>
     <row r="33" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="89"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="101"/>
-      <c r="I33" s="84"/>
-      <c r="J33" s="84"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="135"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="135"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="87" t="s">
+      <c r="B34" s="127" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="90" t="s">
+      <c r="C34" s="130" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="91"/>
-      <c r="E34" s="90" t="s">
+      <c r="D34" s="131"/>
+      <c r="E34" s="130" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="91"/>
-      <c r="G34" s="96" t="s">
+      <c r="F34" s="131"/>
+      <c r="G34" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="H34" s="97"/>
-      <c r="I34" s="82" t="s">
+      <c r="H34" s="103"/>
+      <c r="I34" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="J34" s="82" t="s">
+      <c r="J34" s="99" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="88"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="98"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
+      <c r="B35" s="128"/>
+      <c r="C35" s="132"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="132"/>
+      <c r="F35" s="133"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="105"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="88"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="133"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="133"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="88"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="98"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="132"/>
+      <c r="D37" s="133"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="104"/>
+      <c r="H37" s="105"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="89"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="95"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="95"/>
-      <c r="G38" s="100"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="84"/>
-      <c r="J38" s="84"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="135"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="135"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="107"/>
+      <c r="I38" s="101"/>
+      <c r="J38" s="101"/>
     </row>
     <row r="39" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="127" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="90" t="s">
+      <c r="C39" s="130" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="91"/>
-      <c r="E39" s="90" t="s">
+      <c r="D39" s="131"/>
+      <c r="E39" s="130" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="91"/>
-      <c r="G39" s="96" t="s">
+      <c r="F39" s="131"/>
+      <c r="G39" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="H39" s="97"/>
-      <c r="I39" s="82" t="s">
+      <c r="H39" s="103"/>
+      <c r="I39" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="J39" s="82" t="s">
+      <c r="J39" s="99" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="88"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="93"/>
-      <c r="G40" s="98"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="83"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="132"/>
+      <c r="D40" s="133"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="133"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
     </row>
     <row r="41" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="88"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="93"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="98"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="83"/>
-      <c r="J41" s="83"/>
+      <c r="B41" s="128"/>
+      <c r="C41" s="132"/>
+      <c r="D41" s="133"/>
+      <c r="E41" s="132"/>
+      <c r="F41" s="133"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="105"/>
+      <c r="I41" s="100"/>
+      <c r="J41" s="100"/>
     </row>
     <row r="42" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="88"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="93"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="93"/>
-      <c r="G42" s="98"/>
-      <c r="H42" s="99"/>
-      <c r="I42" s="83"/>
-      <c r="J42" s="83"/>
+      <c r="B42" s="128"/>
+      <c r="C42" s="132"/>
+      <c r="D42" s="133"/>
+      <c r="E42" s="132"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="104"/>
+      <c r="H42" s="105"/>
+      <c r="I42" s="100"/>
+      <c r="J42" s="100"/>
     </row>
     <row r="43" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="89"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="94"/>
-      <c r="F43" s="95"/>
-      <c r="G43" s="100"/>
-      <c r="H43" s="101"/>
-      <c r="I43" s="84"/>
-      <c r="J43" s="84"/>
+      <c r="B43" s="129"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="135"/>
+      <c r="E43" s="134"/>
+      <c r="F43" s="135"/>
+      <c r="G43" s="106"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="101"/>
+      <c r="J43" s="101"/>
     </row>
     <row r="55" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B55" s="56" t="s">
@@ -3927,21 +3930,28 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J29:J33"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C34:D38"/>
+    <mergeCell ref="C39:D43"/>
+    <mergeCell ref="E34:F38"/>
+    <mergeCell ref="E39:F43"/>
+    <mergeCell ref="G34:H38"/>
+    <mergeCell ref="G39:H43"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="I39:I43"/>
+    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="J39:J43"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:D33"/>
+    <mergeCell ref="E29:F33"/>
+    <mergeCell ref="G29:H33"/>
+    <mergeCell ref="E24:F28"/>
+    <mergeCell ref="C24:D28"/>
     <mergeCell ref="J24:J28"/>
     <mergeCell ref="I24:I28"/>
     <mergeCell ref="G24:H28"/>
@@ -3958,28 +3968,21 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:D33"/>
-    <mergeCell ref="E29:F33"/>
-    <mergeCell ref="G29:H33"/>
-    <mergeCell ref="E24:F28"/>
-    <mergeCell ref="C24:D28"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="J29:J33"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C34:D38"/>
-    <mergeCell ref="C39:D43"/>
-    <mergeCell ref="E34:F38"/>
-    <mergeCell ref="E39:F43"/>
-    <mergeCell ref="G34:H38"/>
-    <mergeCell ref="G39:H43"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="I39:I43"/>
-    <mergeCell ref="J34:J38"/>
-    <mergeCell ref="J39:J43"/>
-    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
@@ -4003,7 +4006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -4335,7 +4338,9 @@
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
+      <c r="F32" s="31" t="s">
+        <v>154</v>
+      </c>
       <c r="G32" s="30"/>
       <c r="H32" s="30"/>
       <c r="I32" s="30"/>

</xml_diff>